<commit_message>
Create v1.2 with data format in {key: {dict}}, also added function to check for 403 return of inactive vacancy
</commit_message>
<xml_diff>
--- a/data/Physioswiss Stellen Historisch 23012024-test.xlsx
+++ b/data/Physioswiss Stellen Historisch 23012024-test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="113">
   <si>
     <t>Arbeitgeber</t>
   </si>
@@ -84,13 +84,289 @@
   </si>
   <si>
     <t>Aktiv</t>
+  </si>
+  <si>
+    <t>Actiphysio, associé Christian Wieser &amp; Fabio La Spada</t>
+  </si>
+  <si>
+    <t>Physiotherapie</t>
+  </si>
+  <si>
+    <t>Physiotherapie Andreas Mühlheim GmbH</t>
+  </si>
+  <si>
+    <t>Physiotherapie am Badischen Bahnhof Yvonne Romey</t>
+  </si>
+  <si>
+    <t>Physiozentrum – Uster</t>
+  </si>
+  <si>
+    <t>Time Out Training GmbH</t>
+  </si>
+  <si>
+    <t>Av. de Cerjat  6</t>
+  </si>
+  <si>
+    <t>Romanshornerstr. 10a</t>
+  </si>
+  <si>
+    <t>Ringweg 2</t>
+  </si>
+  <si>
+    <t>Rosentalstrasse 70</t>
+  </si>
+  <si>
+    <t>Poststrasse 7a</t>
+  </si>
+  <si>
+    <t>Bodenstrasse 20</t>
+  </si>
+  <si>
+    <t>Vincent Nijland</t>
+  </si>
+  <si>
+    <t>1510</t>
+  </si>
+  <si>
+    <t>8580</t>
+  </si>
+  <si>
+    <t>3427</t>
+  </si>
+  <si>
+    <t>4058</t>
+  </si>
+  <si>
+    <t>8610</t>
+  </si>
+  <si>
+    <t>6403</t>
+  </si>
+  <si>
+    <t>Moudon</t>
+  </si>
+  <si>
+    <t>Amriswil</t>
+  </si>
+  <si>
+    <t>Utzenstorf</t>
+  </si>
+  <si>
+    <t>Basel</t>
+  </si>
+  <si>
+    <t>Uster</t>
+  </si>
+  <si>
+    <t>Küssnacht</t>
+  </si>
+  <si>
+    <t>Waadt</t>
+  </si>
+  <si>
+    <t>Thurgau</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>Solothurn</t>
+  </si>
+  <si>
+    <t>Basel-Stadt</t>
+  </si>
+  <si>
+    <t>Zürich</t>
+  </si>
+  <si>
+    <t>Schwyz</t>
+  </si>
+  <si>
+    <t>Lausanne</t>
+  </si>
+  <si>
+    <t>St. Gallen</t>
+  </si>
+  <si>
+    <t>Zurich</t>
+  </si>
+  <si>
+    <t>Luzern</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Physiothérapeute 40-100% à Moudon, proche de Lausanne, VAUD.</t>
+  </si>
+  <si>
+    <t>Physiotherapeutin gesucht</t>
+  </si>
+  <si>
+    <t>Dipl. Physiotherapeut/in 50-100%</t>
+  </si>
+  <si>
+    <t>Physiotherapeut*in ca. 60 - 70% angestellt oder selbständig</t>
+  </si>
+  <si>
+    <t>ZentrumsleiterIn 100% für Zentrum in Uster gesucht</t>
+  </si>
+  <si>
+    <t>Physiotherapeut:in im Time Out 80 - 100%</t>
+  </si>
+  <si>
+    <t>40 - 100 %</t>
+  </si>
+  <si>
+    <t>40 - 80 %</t>
+  </si>
+  <si>
+    <t>50 - 100 %</t>
+  </si>
+  <si>
+    <t>60 - 70 %</t>
+  </si>
+  <si>
+    <t>100 %</t>
+  </si>
+  <si>
+    <t>80 - 100 %</t>
+  </si>
+  <si>
+    <t>Sofort</t>
+  </si>
+  <si>
+    <t>Nach Vereinbarung</t>
+  </si>
+  <si>
+    <t>Montag, 1. April 2024</t>
+  </si>
+  <si>
+    <t>Donnerstag, 1. Februar 2024</t>
+  </si>
+  <si>
+    <t>Montag, 1. Januar 2024</t>
+  </si>
+  <si>
+    <t>Festanstellung</t>
+  </si>
+  <si>
+    <t>02-01-2024</t>
+  </si>
+  <si>
+    <t>23-12-2023</t>
+  </si>
+  <si>
+    <t>23-11-2023</t>
+  </si>
+  <si>
+    <t>24-10-2023</t>
+  </si>
+  <si>
+    <t>23-01-2024</t>
+  </si>
+  <si>
+    <t>Herr Fabio La Spada</t>
+  </si>
+  <si>
+    <t>Herr Vincent Nijland</t>
+  </si>
+  <si>
+    <t>Herr Andreas Mühlheim</t>
+  </si>
+  <si>
+    <t>Frau Yvonne Romey</t>
+  </si>
+  <si>
+    <t>Frau Martina Landolt</t>
+  </si>
+  <si>
+    <t>Herr Iwan Kälin</t>
+  </si>
+  <si>
+    <t>0219052618</t>
+  </si>
+  <si>
+    <t>0714117876</t>
+  </si>
+  <si>
+    <t>0326654232</t>
+  </si>
+  <si>
+    <t>0616911366</t>
+  </si>
+  <si>
+    <t>0442713366</t>
+  </si>
+  <si>
+    <t>0415303333</t>
+  </si>
+  <si>
+    <t>0792939516</t>
+  </si>
+  <si>
+    <t>actiphysio@gmail.com</t>
+  </si>
+  <si>
+    <t>nijland.vincent@bluewin.ch</t>
+  </si>
+  <si>
+    <t>physio.muehlheim@bluewin.ch</t>
+  </si>
+  <si>
+    <t>yvonne.romey@physio-hin.ch</t>
+  </si>
+  <si>
+    <t>jobs@physiozentrum.ch</t>
+  </si>
+  <si>
+    <t>iwan@timeout-training.ch</t>
+  </si>
+  <si>
+    <t>http://www.actiphysio-moudon.ch/</t>
+  </si>
+  <si>
+    <t>http://www.kastanienhof.ch/</t>
+  </si>
+  <si>
+    <t>http://www.physio-muehlheim.ch/</t>
+  </si>
+  <si>
+    <t>http://physio-badischer-bahnhof.ch/</t>
+  </si>
+  <si>
+    <t>https://www.physiozentrum.ch/uster/</t>
+  </si>
+  <si>
+    <t>http://www.timeout-training.ch/</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246793/physiotherapeute-40-100-a-moudon-proche-de-lausanne-vaud</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/178640/physiotherapeutin-gesucht</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/244960/dipl-physiotherapeut-in-50-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/244958/dipl-physiotherapeut-in-50-100</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246621/physiotherapeut-in-ca-60-70-angestellt-oder-selbstaendig</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/246523/zentrumsleiterin-100-fuer-zentrum-in-uster-gesucht</t>
+  </si>
+  <si>
+    <t>https://www.physioswiss.ch/de/jobs/243043/physiotherapeut-in-im-time-out-80-100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +381,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,16 +422,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,7 +730,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -512,14 +801,428 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" t="s">
+        <v>88</v>
+      </c>
+      <c r="R3" t="s">
+        <v>95</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" t="s">
+        <v>83</v>
+      </c>
+      <c r="P4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R4" t="s">
+        <v>96</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" t="s">
+        <v>78</v>
+      </c>
+      <c r="N5" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>93</v>
+      </c>
+      <c r="R5" t="s">
+        <v>96</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" t="s">
+        <v>80</v>
+      </c>
+      <c r="O6" t="s">
+        <v>84</v>
+      </c>
+      <c r="P6" t="s">
+        <v>90</v>
+      </c>
+      <c r="R6" t="s">
+        <v>97</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O7" t="s">
+        <v>85</v>
+      </c>
+      <c r="P7" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" t="s">
+        <v>98</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" t="s">
+        <v>86</v>
+      </c>
+      <c r="P8" t="s">
+        <v>92</v>
+      </c>
+      <c r="R8" t="s">
+        <v>99</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+    <hyperlink ref="S4" r:id="rId5"/>
+    <hyperlink ref="T4" r:id="rId6"/>
+    <hyperlink ref="S5" r:id="rId7"/>
+    <hyperlink ref="T5" r:id="rId8"/>
+    <hyperlink ref="S6" r:id="rId9"/>
+    <hyperlink ref="T6" r:id="rId10"/>
+    <hyperlink ref="S7" r:id="rId11"/>
+    <hyperlink ref="T7" r:id="rId12"/>
+    <hyperlink ref="S8" r:id="rId13"/>
+    <hyperlink ref="T8" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -590,14 +1293,74 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
+      <c r="R2" t="s">
+        <v>97</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -668,7 +1431,131 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>78</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>83</v>
+      </c>
+      <c r="P2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="T3" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -753,7 +1640,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -824,14 +1711,71 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -902,14 +1846,74 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" t="s">
+        <v>99</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -980,14 +1984,77 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" t="s">
+        <v>95</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1058,7 +2125,67 @@
         <v>20</v>
       </c>
     </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" t="s">
+        <v>98</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="T2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>